<commit_message>
Correct percentage for f1040 schedule SE line 10
</commit_message>
<xml_diff>
--- a/Federal/f1040sse-2020.xlsx
+++ b/Federal/f1040sse-2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCC\ewc\taxes\tax_worksheets\Federal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Federal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -603,34 +603,10 @@
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -639,16 +615,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -658,6 +630,34 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="A9:F32"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1022,135 +1022,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="5" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
     </row>
     <row r="6" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
     </row>
     <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="31" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="14" t="s">
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="14" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="14" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="9">
         <f>SUM(F9:F12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="14" t="s">
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="9">
         <f>ROUND(IF(F13&gt;0,0.9235*F13,F13),2)</f>
         <v>0</v>
       </c>
@@ -1159,42 +1159,42 @@
       <c r="A15" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="14" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="9">
         <f>F39+F44</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="14" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="9">
         <f>F14+F16</f>
         <v>0</v>
       </c>
@@ -1203,76 +1203,76 @@
       <c r="A18" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="39">
+      <c r="D19" s="5"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="23">
         <f>ROUND(D19*0.9235,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="14" t="s">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="9">
         <f>IF(F19&lt;100,0,F19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="14" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="9">
         <f>F17+F20</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="14" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="9">
         <v>137700</v>
       </c>
     </row>
@@ -1280,504 +1280,504 @@
       <c r="A23" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="14" t="s">
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="9">
         <f>SUM(D24:D26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="14" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="9">
         <f>F22-F27</f>
         <v>137700</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="14" t="s">
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="21">
-        <f>ROUND(0.214 * MIN(F21,F28), 2)</f>
+      <c r="F29" s="9">
+        <f>ROUND(0.124 * MIN(F21,F28), 2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="14" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="9">
         <f>ROUND(0.029*F21,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="14" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="24">
         <f>F30+F29</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="26">
         <f>ROUND(F31/2,2)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="43"/>
-      <c r="F32" s="44"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
     </row>
     <row r="37" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="31" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="18">
         <v>5640</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="14" t="s">
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="21"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="24"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="24"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="24"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="14" t="s">
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="21">
+      <c r="F43" s="9">
         <f>F38-F39</f>
         <v>5640</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="30" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="35"/>
       <c r="D44" s="35"/>
-      <c r="E44" s="27" t="s">
+      <c r="E44" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="36"/>
+      <c r="F44" s="20"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="19"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="14" t="s">
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F52" s="21"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="14" t="s">
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="21">
+      <c r="F53" s="9">
         <f>ROUND(IF(F52&gt;0,0.9235*F52,F52),2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="14" t="s">
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="21"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="14" t="s">
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F55" s="21">
+      <c r="F55" s="9">
         <f>F53+F54</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="22"/>
-      <c r="B56" s="13" t="s">
+      <c r="A56" s="10"/>
+      <c r="B56" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="24"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="14" t="s">
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="21"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="14" t="s">
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F58" s="21">
+      <c r="F58" s="9">
         <f>ROUND(0.2935*F57,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="14" t="s">
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F59" s="21">
+      <c r="F59" s="9">
         <f>F55+F58</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="14" t="s">
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F60" s="21">
+      <c r="F60" s="9">
         <f>MIN(F28,F59)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="27" t="s">
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F61" s="28">
+      <c r="F61" s="15">
         <f>ROUND(F60*0.062,2)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>